<commit_message>
Alles gefixt/ergänzt was wir heute bezüglich der Anforderungsspezifikation besprochen haben + das neue Datenmodell eingefügt
</commit_message>
<xml_diff>
--- a/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/Anwendungsfalltabelle.xlsx
+++ b/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/Anwendungsfalltabelle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Johannes/SE-Project2018/Dokumente/02_Arbeitsbereich/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Johannes/SE-Project2018/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t>Akteur</t>
   </si>
@@ -47,19 +47,10 @@
     <t>2/Spiel laden</t>
   </si>
   <si>
-    <t>Umsetzung in Aktivitätsdiagramm</t>
-  </si>
-  <si>
     <t>3/ Spiel starten</t>
   </si>
   <si>
     <t>4/ Spiel beenden</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>Nein</t>
   </si>
   <si>
     <t>Beenden des Spiels
@@ -90,30 +81,11 @@
     <t>Client</t>
   </si>
   <si>
-    <t>5/ Anmelden</t>
-  </si>
-  <si>
     <t>8/ Spielzug
       durchführen</t>
   </si>
   <si>
-    <t>9/ Phase I</t>
-  </si>
-  <si>
-    <t>10/ Phase II</t>
-  </si>
-  <si>
-    <t>11/ Phase III</t>
-  </si>
-  <si>
-    <t>12/ Abwehr</t>
-  </si>
-  <si>
     <t>6/ Bereit melden</t>
-  </si>
-  <si>
-    <t>7/ Studenten 
-      Verteilen</t>
   </si>
   <si>
     <t>Anmelden am Server
@@ -151,6 +123,110 @@
   <si>
     <t>Angriff von anderem
 Spieler abwehren</t>
+  </si>
+  <si>
+    <t>5/ Am Server
+      anmelden</t>
+  </si>
+  <si>
+    <t>7/ Ersties 
+      verteilen</t>
+  </si>
+  <si>
+    <t>9/ Phase I
+     durchführen</t>
+  </si>
+  <si>
+    <t>10/ Phase II
+        durchführen</t>
+  </si>
+  <si>
+    <t>11/ Phase III
+        durchführen</t>
+  </si>
+  <si>
+    <t>12/ Angriff
+        abwehren</t>
+  </si>
+  <si>
+    <t>Vorbedingung</t>
+  </si>
+  <si>
+    <t>Server ist 
+gestartet 
+und es wurde
+neues Spiel
+gewählt</t>
+  </si>
+  <si>
+    <t>Server ist 
+gestartet 
+und es wurde
+Spiel laden
+gewählt</t>
+  </si>
+  <si>
+    <t>ID 1 oder ID 2 abgeschlossen.
+Im Fall ID 2:
+Name und
+Pw der
+geladenen 
+Partie immer noch bekannt</t>
+  </si>
+  <si>
+    <t>ID 1 oder ID 2 
+und ID 6
+abgeschlossen</t>
+  </si>
+  <si>
+    <t>ID 5
+abgeschlossen</t>
+  </si>
+  <si>
+    <t>ID 3
+abgeschlossen</t>
+  </si>
+  <si>
+    <t>Spiel läuft und 
+ID 8
+abgeschlossen</t>
+  </si>
+  <si>
+    <t>ID 8 
+begonnen</t>
+  </si>
+  <si>
+    <t>ID 9
+abgeschlossen</t>
+  </si>
+  <si>
+    <t>ID 10
+abgeschlossen</t>
+  </si>
+  <si>
+    <t>Ein Client in
+ID 10 greift
+ein Gebäude
+des Akteurs an</t>
+  </si>
+  <si>
+    <t>ID 7 
+abgeschlossen
+und Akteur
+ist an der
+Reihe</t>
+  </si>
+  <si>
+    <t>Aufrufhäufigkeit</t>
+  </si>
+  <si>
+    <t>Sehr gering</t>
+  </si>
+  <si>
+    <t>Sehr häufig</t>
+  </si>
+  <si>
+    <t>Häufig</t>
   </si>
 </sst>
 </file>
@@ -231,7 +307,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -239,8 +315,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -257,16 +339,28 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,23 +636,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:H6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -569,22 +664,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -592,25 +678,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -618,143 +695,209 @@
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="D4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="D6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="D13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>